<commit_message>
updated SIL+AUC database export
</commit_message>
<xml_diff>
--- a/data/escapement/prelim-inseason/2025/EscEstSppHeader.xlsx
+++ b/data/escapement/prelim-inseason/2025/EscEstSppHeader.xlsx
@@ -1665,16 +1665,16 @@
         <v>0</v>
       </c>
       <c r="AA10" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB10" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="0">
         <v>0</v>
       </c>
       <c r="AD10" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AE10" s="0">
         <v>0</v>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="AM10" s="0" t="inlineStr">
         <is>
-          <t>Two full system swims conducted, but split over two days each: USJ Oct 6, LSJ Oct 7, USJ Oct 16, LSJ Oct 17, USJ Dec 1, LSJ Dec 3. Grouped swims together manually based on first day of swims (6, 16, 1). Very good conditions on all swims. Used expanded PL+D.Type-4 due to three swims.</t>
+          <t>Two full system swims conducted, but split over two days each: USJ Oct 6, LSJ Oct 7, USJ Oct 16, LSJ Oct 17, USJ Dec 1, LSJ Dec 3. Grouped swims together manually based on first day of swims (6, 16, 1). Very good conditions on all swims. Fence counts passed 10 pinks over the fence so adopted the unexpanded estimate of 10 pinks this year (only 4 seen on swims).</t>
         </is>
       </c>
       <c r="AN10" s="0" t="b">

</xml_diff>